<commit_message>
update and fished work with excel export
</commit_message>
<xml_diff>
--- a/grails-app/base/templates/documentBase.xlsx
+++ b/grails-app/base/templates/documentBase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">KUSTOMER</t>
   </si>
@@ -55,34 +55,7 @@
     <t xml:space="preserve">FECHA TERMINO</t>
   </si>
   <si>
-    <t xml:space="preserve">PRESUPUESTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAREAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESTADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARTICIPANTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOBMRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APELLIDOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORREO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIRECCION</t>
+    <t xml:space="preserve">CREADO POR</t>
   </si>
 </sst>
 </file>
@@ -123,6 +96,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -136,7 +110,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +121,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -184,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,7 +177,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,8 +185,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -218,6 +206,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -225,16 +273,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>812160</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3230640</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>193320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>516240</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>429840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -247,8 +295,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3415320" y="193320"/>
-          <a:ext cx="1005840" cy="936720"/>
+          <a:off x="4564080" y="193320"/>
+          <a:ext cx="1225080" cy="933840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -268,16 +316,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="18.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.0561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.780612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,7 +340,6 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
       <c r="G1" s="0" t="s">
         <v>1</v>
       </c>
@@ -309,162 +360,117 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>11</v>
-      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>